<commit_message>
Changed USB to differential pair
</commit_message>
<xml_diff>
--- a/Baud calcs.xlsx
+++ b/Baud calcs.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>BRG16</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>Actual Baud</t>
+  </si>
+  <si>
+    <t>Bits per channel</t>
+  </si>
+  <si>
+    <t>Channels per card</t>
+  </si>
+  <si>
+    <t>Cards</t>
+  </si>
+  <si>
+    <t>Bits per sample</t>
+  </si>
+  <si>
+    <t>Bytes per sample</t>
   </si>
 </sst>
 </file>
@@ -53,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -86,8 +101,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -373,14 +388,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -470,6 +487,48 @@
       <c r="D7">
         <f>Fosc/(4*(ROUND(C7,0)+1))</f>
         <v>115384.61538461539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <f>B12*B13*B14</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <f>B15/8</f>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>